<commit_message>
GPLIM-2957: fix excel headers so they match with values in Decision:  https://labopsconfluence.broadinstitute.org/pages/viewpage.action?pageId=22676493
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/manifest-import/test-manifest-duplicate-columns.xlsx
+++ b/mercury/src/test/resources/testdata/manifest-import/test-manifest-duplicate-columns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="280" windowWidth="25600" windowHeight="20460"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="Buick Example" sheetId="2" r:id="rId1"/>
@@ -246,12 +246,6 @@
     <t>24-Apr-2012</t>
   </si>
   <si>
-    <t>T/N</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -262,6 +256,12 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>SAMPLE_TYPE</t>
+  </si>
+  <si>
+    <t>Specimen_Number</t>
   </si>
 </sst>
 </file>
@@ -322,8 +322,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -343,9 +345,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -746,7 +750,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -760,7 +764,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -778,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -792,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -801,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -815,7 +819,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -824,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -838,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -847,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -861,7 +865,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -870,7 +874,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -884,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
@@ -893,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -907,7 +911,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
@@ -916,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -930,7 +934,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>25</v>
@@ -939,7 +943,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -953,7 +957,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>28</v>
@@ -962,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -976,7 +980,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
@@ -985,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -999,7 +1003,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -1008,7 +1012,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1022,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>37</v>
@@ -1031,7 +1035,7 @@
         <v>7</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1045,7 +1049,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
@@ -1054,7 +1058,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1068,7 +1072,7 @@
         <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>43</v>
@@ -1077,7 +1081,7 @@
         <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1091,7 +1095,7 @@
         <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>46</v>
@@ -1100,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1114,7 +1118,7 @@
         <v>48</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>49</v>
@@ -1123,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1137,7 +1141,7 @@
         <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>52</v>
@@ -1146,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1160,7 +1164,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>55</v>
@@ -1169,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1183,7 +1187,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>58</v>
@@ -1192,7 +1196,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1206,7 +1210,7 @@
         <v>60</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>61</v>
@@ -1215,7 +1219,7 @@
         <v>7</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1229,7 +1233,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>64</v>
@@ -1238,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1252,7 +1256,7 @@
         <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>67</v>
@@ -1261,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1275,7 +1279,7 @@
         <v>69</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>70</v>
@@ -1284,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1298,7 +1302,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>73</v>
@@ -1307,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>